<commit_message>
bug push to fix
</commit_message>
<xml_diff>
--- a/Databases/中文_words.xlsx
+++ b/Databases/中文_words.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="185">
   <si>
     <t>FOREIGN</t>
   </si>
@@ -245,6 +245,45 @@
   </si>
   <si>
     <t>提倡</t>
+  </si>
+  <si>
+    <t>骚扰</t>
+  </si>
+  <si>
+    <t>气不忿儿</t>
+  </si>
+  <si>
+    <t>煽动者</t>
+  </si>
+  <si>
+    <t>初衷</t>
+  </si>
+  <si>
+    <t>节约</t>
+  </si>
+  <si>
+    <t>助力</t>
+  </si>
+  <si>
+    <t>推动</t>
+  </si>
+  <si>
+    <t>制止</t>
+  </si>
+  <si>
+    <t>歉意</t>
+  </si>
+  <si>
+    <t>周全</t>
+  </si>
+  <si>
+    <t>完善</t>
+  </si>
+  <si>
+    <t>精准</t>
+  </si>
+  <si>
+    <t>搭配</t>
   </si>
   <si>
     <t>1.) n. catering;
@@ -482,6 +521,45 @@
     <t>1.) n. promotion, advocacy; 2.) v. promote, advocate</t>
   </si>
   <si>
+    <t>1.) vt. harass</t>
+  </si>
+  <si>
+    <t>1.) v. be jealous, take another's success badly; 2.) v. be unable to contain one's anger</t>
+  </si>
+  <si>
+    <t>1.) n. demagogue</t>
+  </si>
+  <si>
+    <t>1.) n. original intent/aspiration</t>
+  </si>
+  <si>
+    <t>1.) v. economize, conserve; 2.) adj. frugal, economic</t>
+  </si>
+  <si>
+    <t>1.) n. a helping hand, help, assistance</t>
+  </si>
+  <si>
+    <t>1.) v. push forward, promote, to push [for acceptance], to actuate</t>
+  </si>
+  <si>
+    <t>1.) v. put a stop to, curb, to check, to limit</t>
+  </si>
+  <si>
+    <t>1.) n. apology; 2.) regret</t>
+  </si>
+  <si>
+    <t>1.) adj. thorough, comprehensive</t>
+  </si>
+  <si>
+    <t>1.) v. to perfect, to improve; 2.) adj. perfect</t>
+  </si>
+  <si>
+    <t>1.) adj. accurate, precise, exact; 2.) precision, accuracy</t>
+  </si>
+  <si>
+    <t>1.) v. pair up, match, arrange in pairs, add sth into a group</t>
+  </si>
+  <si>
     <t>2020-11-25</t>
   </si>
   <si>
@@ -501,6 +579,9 @@
   </si>
   <si>
     <t>2020-12-03</t>
+  </si>
+  <si>
+    <t>2020-12-04</t>
   </si>
 </sst>
 </file>
@@ -858,7 +939,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -880,10 +961,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -891,10 +972,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -902,10 +983,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -913,10 +994,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -924,10 +1005,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -935,10 +1016,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -946,10 +1027,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -957,10 +1038,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -968,10 +1049,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -979,10 +1060,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -990,10 +1071,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1001,10 +1082,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1012,10 +1093,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1023,10 +1104,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1034,10 +1115,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1045,10 +1126,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1056,10 +1137,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1067,10 +1148,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1078,10 +1159,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1089,10 +1170,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1100,10 +1181,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1111,10 +1192,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1122,10 +1203,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1133,10 +1214,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1144,10 +1225,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1155,10 +1236,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1166,10 +1247,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1177,10 +1258,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1188,10 +1269,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1199,10 +1280,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C31" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1210,10 +1291,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C32" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1221,10 +1302,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1232,10 +1313,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1243,10 +1324,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1254,10 +1335,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="C36" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1265,10 +1346,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1276,10 +1357,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1287,10 +1368,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1298,10 +1379,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1309,10 +1390,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C41" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1320,10 +1401,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1331,10 +1412,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1342,10 +1423,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1353,10 +1434,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1364,10 +1445,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1375,10 +1456,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="C47" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1386,10 +1467,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1397,10 +1478,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1408,10 +1489,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1419,10 +1500,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="C51" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1430,10 +1511,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1441,10 +1522,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C53" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1452,10 +1533,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1463,10 +1544,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1474,10 +1555,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C56" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1485,10 +1566,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C57" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1496,10 +1577,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1507,10 +1588,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C59" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1518,10 +1599,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1529,10 +1610,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1540,10 +1621,10 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1551,10 +1632,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1562,10 +1643,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1573,10 +1654,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1584,10 +1665,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="C66" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1595,10 +1676,10 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C67" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1606,10 +1687,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="C68" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1617,10 +1698,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1628,10 +1709,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="C70" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1639,10 +1720,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1650,10 +1731,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="C72" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1661,10 +1742,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="C73" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1672,10 +1753,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="C74" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1683,10 +1764,153 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" t="s">
+        <v>164</v>
+      </c>
+      <c r="C76" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" t="s">
+        <v>170</v>
+      </c>
+      <c r="C82" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updatedDBs and added issue #22
</commit_message>
<xml_diff>
--- a/Databases/中文_words.xlsx
+++ b/Databases/中文_words.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="192">
   <si>
     <t>FOREIGN</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>搭配</t>
+  </si>
+  <si>
+    <t>保留</t>
+  </si>
+  <si>
+    <t>授予</t>
+  </si>
+  <si>
+    <t>诺贝尔</t>
   </si>
   <si>
     <t>1.) n. catering;
@@ -560,6 +569,15 @@
     <t>1.) v. pair up, match, arrange in pairs, add sth into a group</t>
   </si>
   <si>
+    <t>1.) v. preserve, hold back, retain, reserve</t>
+  </si>
+  <si>
+    <t>1.) vt. award, confer, grand, endow</t>
+  </si>
+  <si>
+    <t>1.) Nobel Prize</t>
+  </si>
+  <si>
     <t>2020-11-25</t>
   </si>
   <si>
@@ -582,6 +600,9 @@
   </si>
   <si>
     <t>2020-12-04</t>
+  </si>
+  <si>
+    <t>2020-12-08</t>
   </si>
 </sst>
 </file>
@@ -939,7 +960,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -961,10 +982,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -972,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -983,10 +1004,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -994,10 +1015,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1005,10 +1026,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1016,10 +1037,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1027,10 +1048,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1038,10 +1059,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1049,10 +1070,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1060,10 +1081,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1071,10 +1092,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1082,10 +1103,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1093,10 +1114,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1104,10 +1125,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1115,10 +1136,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1126,10 +1147,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1137,10 +1158,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1148,10 +1169,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1159,10 +1180,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1170,10 +1191,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1181,10 +1202,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1192,10 +1213,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1203,10 +1224,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1214,10 +1235,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1225,10 +1246,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1236,10 +1257,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1247,10 +1268,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C28" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1258,10 +1279,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C29" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1269,10 +1290,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1280,10 +1301,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1291,10 +1312,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C32" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1302,10 +1323,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1313,10 +1334,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1324,10 +1345,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C35" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1335,10 +1356,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1346,10 +1367,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1357,10 +1378,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C38" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1368,10 +1389,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C39" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1379,10 +1400,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1390,10 +1411,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1401,10 +1422,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C42" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1412,10 +1433,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C43" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1423,10 +1444,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1434,10 +1455,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C45" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1445,10 +1466,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C46" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1456,10 +1477,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C47" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1467,10 +1488,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C48" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1478,10 +1499,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C49" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1489,10 +1510,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C50" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1500,10 +1521,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1511,10 +1532,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1522,10 +1543,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C53" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1533,10 +1554,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C54" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1544,10 +1565,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1555,10 +1576,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C56" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1566,10 +1587,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1577,10 +1598,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C58" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1588,10 +1609,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1599,10 +1620,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C60" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1610,10 +1631,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C61" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1621,10 +1642,10 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C62" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1632,10 +1653,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1643,10 +1664,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1654,10 +1675,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C65" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1665,10 +1686,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C66" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1676,10 +1697,10 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C67" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1687,10 +1708,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C68" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1698,10 +1719,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C69" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1709,10 +1730,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C70" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1720,10 +1741,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C71" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1731,10 +1752,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C72" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1742,10 +1763,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1753,10 +1774,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C74" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1764,10 +1785,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C75" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1775,10 +1796,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C76" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1786,10 +1807,10 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1797,10 +1818,10 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C78" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1808,10 +1829,10 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C79" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1819,10 +1840,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C80" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1830,10 +1851,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C81" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1841,10 +1862,10 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C82" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1852,10 +1873,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C83" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1863,10 +1884,10 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C84" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1874,10 +1895,10 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C85" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1885,10 +1906,10 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C86" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1896,10 +1917,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C87" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1907,10 +1928,43 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" t="s">
+        <v>182</v>
+      </c>
+      <c r="C91" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>